<commit_message>
continue generation XLSX file
</commit_message>
<xml_diff>
--- a/templates/files/ind_plan_example.xlsx
+++ b/templates/files/ind_plan_example.xlsx
@@ -664,37 +664,36 @@
   <dimension ref="A1:AMI21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="2.83673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="3.64285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="5.12755102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="4.45408163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="2.69897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.0255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="11.5918367346939"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="3.37244897959184"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="3.64285714285714"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="3.51020408163265"/>
     <col collapsed="false" hidden="false" max="25" min="17" style="1" width="3.23979591836735"/>
-    <col collapsed="false" hidden="false" max="27" min="26" style="1" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="27" min="26" style="1" width="3.91326530612245"/>
     <col collapsed="false" hidden="false" max="40" min="28" style="1" width="3.23979591836735"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="1" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="1" width="4.05102040816327"/>
     <col collapsed="false" hidden="false" max="45" min="42" style="1" width="3.23979591836735"/>
-    <col collapsed="false" hidden="false" max="47" min="46" style="1" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="47" min="46" style="1" width="3.91326530612245"/>
     <col collapsed="false" hidden="false" max="65" min="48" style="1" width="3.23979591836735"/>
-    <col collapsed="false" hidden="false" max="67" min="66" style="1" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="67" min="66" style="1" width="3.91326530612245"/>
     <col collapsed="false" hidden="false" max="69" min="68" style="1" width="3.23979591836735"/>
-    <col collapsed="false" hidden="false" max="1023" min="70" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1023" min="70" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2592,29 +2591,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="2.83673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="3" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="2.69897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="3" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="9.71938775510204"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="3" width="3.37244897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="3" width="3.64285714285714"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="3" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="3" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="5.66836734693878"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="3" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="3" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="3" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="3" width="5.53571428571429"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="3" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="3" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="3" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="3" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="26" min="24" style="3" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="3" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="1021" min="28" style="3" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="3" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="3" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="3" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="26" min="24" style="3" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="3" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="1021" min="28" style="3" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3903,10 +3901,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="14" min="3" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="14" min="3" style="0" width="5.26530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4104,11 +4100,10 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.12755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.1428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4165,12 +4160,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4229,12 +4223,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4286,12 +4279,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>